<commit_message>
update 21 aug 2023, add tong_cyber
</commit_message>
<xml_diff>
--- a/player/checked/20230821_listplayer.xlsx
+++ b/player/checked/20230821_listplayer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1dd2fc4bf918acb/Projects/badminton-payment2/player/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d1dd2fc4bf918acb/Projects/badminton-payment2/player/checked/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{4EB981FD-41DE-5B48-84AA-4FE05636D6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E60A8FEA-3FD1-9244-BED3-047FDC357929}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{4EB981FD-41DE-5B48-84AA-4FE05636D6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BB5942A-0E32-413E-AD70-C9D64C678F04}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2023xxxx_listplayer" sheetId="1" r:id="rId1"/>
@@ -1158,26 +1158,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.5" customWidth="1"/>
-    <col min="6" max="6" width="8.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="13" max="13" width="19.5" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1234,7 +1234,7 @@
       </c>
       <c r="E2">
         <f>IF(D2&gt;0, $M$2*D2, 0)</f>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1257,14 +1257,14 @@
       </c>
       <c r="L2">
         <f>SUM(D2:D307)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M2">
         <f>ROUNDUP(K2/L2,0)</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1280,13 +1280,13 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E65" si="1">IF(D3&gt;0, $M$2*D3, 0)</f>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1324,13 +1324,13 @@
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1412,13 +1412,13 @@
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1500,13 +1500,13 @@
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1522,13 +1522,13 @@
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1588,13 +1588,13 @@
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1610,13 +1610,13 @@
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1632,13 +1632,13 @@
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1654,13 +1654,13 @@
       </c>
       <c r="E20">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -1808,13 +1808,13 @@
       </c>
       <c r="E27">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
@@ -1962,13 +1962,13 @@
       </c>
       <c r="E34">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>91</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>91</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -2050,13 +2050,13 @@
       </c>
       <c r="E38">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F38">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>13</v>
       </c>
@@ -2094,13 +2094,13 @@
       </c>
       <c r="E40">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>88</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>88</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -2160,13 +2160,13 @@
       </c>
       <c r="E43">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F43">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>14</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>15</v>
       </c>
@@ -2266,17 +2266,17 @@
         <v>TongCyber</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="F48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>16</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -2336,13 +2336,13 @@
       </c>
       <c r="E51">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>18</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>19</v>
       </c>
@@ -2424,13 +2424,13 @@
       </c>
       <c r="E55">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F55">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>19</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>20</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>21</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>21</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>21</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>21</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>21</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>82</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>85</v>
       </c>
@@ -2644,7 +2644,7 @@
       </c>
       <c r="E65">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F65">
         <v>0</v>

</xml_diff>